<commit_message>
accomodate numeric values for circuit_voltage by automatically appending the necessary 'V'
</commit_message>
<xml_diff>
--- a/tests/_data/test_case_1.xlsx
+++ b/tests/_data/test_case_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="156">
   <si>
     <t xml:space="preserve">Plant Parent ID</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">55_1-1019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accelerator</t>
   </si>
   <si>
     <t xml:space="preserve">FM-58_1-1019-Lathe Disc.</t>
@@ -731,9 +734,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304200</xdr:colOff>
+      <xdr:colOff>303840</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>304200</xdr:rowOff>
+      <xdr:rowOff>303840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -745,7 +748,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="304200" cy="304200"/>
+          <a:ext cx="303840" cy="303840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -774,8 +777,8 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O43" activeCellId="0" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -885,192 +888,264 @@
       <c r="E2" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>30</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>480</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1079,85 +1154,121 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B15" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="B16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T17" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T18" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
+      <c r="F19" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <v>480</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
@@ -1165,141 +1276,201 @@
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T20" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T21" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T22" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T23" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T24" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T25" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T26" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T27" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F28" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T28" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
+      <c r="F29" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T29" s="0" t="n">
+        <v>480</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6"/>
@@ -1307,6 +1478,12 @@
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
+      <c r="F30" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T30" s="0" t="n">
+        <v>480</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6"/>
@@ -1314,346 +1491,478 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F31" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T31" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T32" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T33" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T34" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T35" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T36" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T37" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T38" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="6" t="s">
-        <v>114</v>
-      </c>
       <c r="B39" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T39" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F40" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T40" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F41" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T41" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F42" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T42" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B43" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T43" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="6" t="s">
-        <v>121</v>
-      </c>
       <c r="B44" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F44" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T44" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T45" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T46" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T47" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T48" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C49" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T49" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D49" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>141</v>
-      </c>
       <c r="C50" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>143</v>
-      </c>
       <c r="E50" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+      <c r="F50" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T50" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D51" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T51" s="0" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>146</v>
-      </c>
       <c r="D52" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="T52" s="0" t="n">
+        <v>480</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
@@ -1661,10 +1970,10 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
@@ -1672,10 +1981,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
@@ -1683,10 +1992,10 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
@@ -1694,10 +2003,10 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
@@ -1705,10 +2014,10 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -1716,10 +2025,10 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>

</xml_diff>